<commit_message>
dokumentace a odevzdání 4. iterace
</commit_message>
<xml_diff>
--- a/K odevzdání/Přerozdělení bodů.xlsx
+++ b/K odevzdání/Přerozdělení bodů.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>6.týden</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Další vývoj aplikace + opravy chyb předchozí iterace.</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1083,8 @@
   <dimension ref="A2:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1171,11 +1175,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="29"/>
-      <c r="I4" s="30"/>
+      <c r="I4" s="30">
+        <v>-3</v>
+      </c>
       <c r="J4" s="31"/>
       <c r="K4" s="32">
         <f t="shared" ref="K4:K9" si="0">C4+E4+G4+I4</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1">
@@ -1197,11 +1203,13 @@
         <v>-1</v>
       </c>
       <c r="H5" s="40"/>
-      <c r="I5" s="41"/>
+      <c r="I5" s="41">
+        <v>2</v>
+      </c>
       <c r="J5" s="42"/>
       <c r="K5" s="43">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1">
@@ -1221,11 +1229,13 @@
         <v>-3</v>
       </c>
       <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
+      <c r="I6" s="41">
+        <v>2</v>
+      </c>
       <c r="J6" s="42"/>
       <c r="K6" s="43">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1" thickBot="1">
@@ -1249,11 +1259,13 @@
         <v>3</v>
       </c>
       <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
+      <c r="I7" s="52">
+        <v>-1</v>
+      </c>
       <c r="J7" s="53"/>
       <c r="K7" s="54">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17.25" customHeight="1" thickBot="1">
@@ -1306,16 +1318,18 @@
         <v>19</v>
       </c>
       <c r="G9" s="68">
-        <v>0</v>
-      </c>
-      <c r="H9" s="69"/>
+        <v>4</v>
+      </c>
+      <c r="H9" s="69" t="s">
+        <v>21</v>
+      </c>
       <c r="I9" s="68">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J9" s="70"/>
       <c r="K9" s="71">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:11" hidden="1">

</xml_diff>